<commit_message>
Deploying to gh-pages from @ Healthedata1/USCDI4-Sandbox@b91954a8dc756b73b6d41f6a77ea5acb61d9ea4d 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-us-core-observation-lab.xlsx
+++ b/StructureDefinition-us-core-observation-lab.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="420">
   <si>
     <t>Property</t>
   </si>
@@ -842,7 +842,7 @@
     <t>For some results, particularly numeric results, an interpretation is necessary to fully understand the significance of a result.</t>
   </si>
   <si>
-    <t>Codes identifying interpretations of observations.</t>
+    <t>Observation Interpretation Codes</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-interpretation</t>
@@ -1328,6 +1328,9 @@
   </si>
   <si>
     <t>Historically used for laboratory results (known as 'abnormal flag' ),  its use extends to other use cases where coded interpretations  are relevant.  Often reported as one or more simple compact codes this element is often placed adjacent to the result value in reports and flow sheets to signal the meaning/normalcy status of the result.</t>
+  </si>
+  <si>
+    <t>Codes identifying interpretations of observations.</t>
   </si>
   <si>
     <t>Observation.component.referenceRange</t>
@@ -7684,7 +7687,7 @@
         <v>167</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>260</v>
+        <v>415</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>261</v>
@@ -7740,10 +7743,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7769,13 +7772,13 @@
         <v>39</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>317</v>
@@ -7827,7 +7830,7 @@
         <v>38</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>36</v>

</xml_diff>